<commit_message>
update PAR and a more labeling on units
</commit_message>
<xml_diff>
--- a/Studies/Oregon_Site/Journals-YearlyComparisons/Results_DF_tomato.xlsx
+++ b/Studies/Oregon_Site/Journals-YearlyComparisons/Results_DF_tomato.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sayala\Documents\GitHub\InSPIRE\Studies\Oregon_Site\Journals-YearlyComparisons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F406C8EE-BEE0-4126-AB4C-674A470D8816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51698C4A-316B-4460-9F66-A19B1ACAF49C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,11 +16,11 @@
     <sheet name="Results_DF_tomato" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Results_DF_tomato!$D$15:$D$18</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Results_DF_tomato!$E$14</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Results_DF_tomato!$E$15:$E$18</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Results_DF_tomato!$F$14</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Results_DF_tomato!$F$15:$F$18</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Results_DF_tomato!$D$18:$D$21</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Results_DF_tomato!$E$17</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Results_DF_tomato!$E$18:$E$21</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Results_DF_tomato!$F$17</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Results_DF_tomato!$F$18:$F$21</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="86">
   <si>
     <t>Year</t>
   </si>
@@ -246,60 +246,6 @@
     <t>5.913478530592672</t>
   </si>
   <si>
-    <t>2020_GHI</t>
-  </si>
-  <si>
-    <t>2020_GroundCoordY</t>
-  </si>
-  <si>
-    <t>2020_Gground</t>
-  </si>
-  <si>
-    <t>2020_Gfront</t>
-  </si>
-  <si>
-    <t>2020_Grear</t>
-  </si>
-  <si>
-    <t>2020_BGG</t>
-  </si>
-  <si>
-    <t>2020_BedA</t>
-  </si>
-  <si>
-    <t>2020_BedB</t>
-  </si>
-  <si>
-    <t>2020_BedC</t>
-  </si>
-  <si>
-    <t>TMY_GHI</t>
-  </si>
-  <si>
-    <t>TMY_GroundCoordY</t>
-  </si>
-  <si>
-    <t>TMY_Gground</t>
-  </si>
-  <si>
-    <t>TMY_Gfront</t>
-  </si>
-  <si>
-    <t>TMY_Grear</t>
-  </si>
-  <si>
-    <t>TMY_BGG</t>
-  </si>
-  <si>
-    <t>TMY_BedA</t>
-  </si>
-  <si>
-    <t>TMY_BedB</t>
-  </si>
-  <si>
-    <t>TMY_BedC</t>
-  </si>
-  <si>
     <t>Difference in GHI</t>
   </si>
   <si>
@@ -319,13 +265,46 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>TMY</t>
+  </si>
+  <si>
+    <t>SETUP 3</t>
+  </si>
+  <si>
+    <t>UNITS FOR GHI, Bed A-C are Monthly or Seasonal Insolation (Wh/m2), as it is the irradiance received integrated over that period of time.</t>
+  </si>
+  <si>
+    <t>GroundCoordY</t>
+  </si>
+  <si>
+    <t>Gground</t>
+  </si>
+  <si>
+    <t>Gfront</t>
+  </si>
+  <si>
+    <t>Grear</t>
+  </si>
+  <si>
+    <t>BGG</t>
+  </si>
+  <si>
+    <t>BedA</t>
+  </si>
+  <si>
+    <t>BedB</t>
+  </si>
+  <si>
+    <t>BedC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -468,8 +447,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -649,6 +636,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -810,7 +803,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
@@ -819,6 +812,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -943,11 +944,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Results_DF_tomato!$L$1</c:f>
+              <c:f>Results_DF_tomato!$L$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2020_BedA</c:v>
+                  <c:v>BedA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -967,7 +968,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Results_DF_tomato!$D$2:$D$8</c:f>
+              <c:f>Results_DF_tomato!$D$5:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -997,7 +998,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Results_DF_tomato!$L$2:$L$8</c:f>
+              <c:f>Results_DF_tomato!$L$5:$L$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1036,11 +1037,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Results_DF_tomato!$M$1</c:f>
+              <c:f>Results_DF_tomato!$M$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2020_BedB</c:v>
+                  <c:v>BedB</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1060,7 +1061,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Results_DF_tomato!$D$2:$D$8</c:f>
+              <c:f>Results_DF_tomato!$D$5:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1090,7 +1091,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Results_DF_tomato!$M$2:$M$8</c:f>
+              <c:f>Results_DF_tomato!$M$5:$M$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1129,11 +1130,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Results_DF_tomato!$N$1</c:f>
+              <c:f>Results_DF_tomato!$N$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2020_BedC</c:v>
+                  <c:v>BedC</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1153,7 +1154,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Results_DF_tomato!$D$2:$D$8</c:f>
+              <c:f>Results_DF_tomato!$D$5:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1183,7 +1184,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Results_DF_tomato!$N$2:$N$8</c:f>
+              <c:f>Results_DF_tomato!$N$5:$N$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1222,11 +1223,11 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Results_DF_tomato!$U$1</c:f>
+              <c:f>Results_DF_tomato!$U$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TMY_BedA</c:v>
+                  <c:v>BedA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1246,7 +1247,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Results_DF_tomato!$D$2:$D$8</c:f>
+              <c:f>Results_DF_tomato!$D$5:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1276,7 +1277,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Results_DF_tomato!$U$2:$U$8</c:f>
+              <c:f>Results_DF_tomato!$U$5:$U$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1315,11 +1316,11 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Results_DF_tomato!$V$1</c:f>
+              <c:f>Results_DF_tomato!$V$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TMY_BedB</c:v>
+                  <c:v>BedB</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1339,7 +1340,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Results_DF_tomato!$D$2:$D$8</c:f>
+              <c:f>Results_DF_tomato!$D$5:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1369,7 +1370,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Results_DF_tomato!$V$2:$V$8</c:f>
+              <c:f>Results_DF_tomato!$V$5:$V$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1408,11 +1409,11 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Results_DF_tomato!$W$1</c:f>
+              <c:f>Results_DF_tomato!$W$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TMY_BedC</c:v>
+                  <c:v>BedC</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1432,7 +1433,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Results_DF_tomato!$D$2:$D$8</c:f>
+              <c:f>Results_DF_tomato!$D$5:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1462,7 +1463,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Results_DF_tomato!$W$2:$W$8</c:f>
+              <c:f>Results_DF_tomato!$W$5:$W$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2998,13 +2999,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>166687</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3034,13 +3035,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>185737</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>600074</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>61912</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3106,6 +3107,67 @@
         </xdr:sp>
       </mc:Fallback>
     </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0EEEF01-2D1D-7912-158E-52059DA64230}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12706350" y="4257675"/>
+          <a:ext cx="1000125" cy="1552575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3408,10 +3470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W18"/>
+  <dimension ref="A1:Y21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3419,290 +3481,110 @@
     <col min="11" max="11" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B1" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A3" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" s="7">
+        <v>2020</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="Y3" s="3"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L1" t="s">
-        <v>74</v>
-      </c>
-      <c r="M1" t="s">
-        <v>75</v>
-      </c>
-      <c r="N1" t="s">
-        <v>76</v>
-      </c>
-      <c r="O1" t="s">
-        <v>77</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
         <v>78</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="H4" t="s">
         <v>79</v>
       </c>
-      <c r="R1" t="s">
+      <c r="I4" t="s">
         <v>80</v>
       </c>
-      <c r="S1" t="s">
+      <c r="J4" t="s">
         <v>81</v>
       </c>
-      <c r="T1" t="s">
+      <c r="K4" t="s">
         <v>82</v>
       </c>
-      <c r="U1" t="s">
+      <c r="L4" t="s">
         <v>83</v>
       </c>
-      <c r="V1" t="s">
+      <c r="M4" t="s">
         <v>84</v>
       </c>
-      <c r="W1" t="s">
+      <c r="N4" t="s">
         <v>85</v>
       </c>
+      <c r="O4" t="s">
+        <v>4</v>
+      </c>
+      <c r="P4" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>79</v>
+      </c>
+      <c r="R4" t="s">
+        <v>80</v>
+      </c>
+      <c r="S4" t="s">
+        <v>81</v>
+      </c>
+      <c r="T4" t="s">
+        <v>82</v>
+      </c>
+      <c r="U4" t="s">
+        <v>83</v>
+      </c>
+      <c r="V4" t="s">
+        <v>84</v>
+      </c>
+      <c r="W4" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>0</v>
-      </c>
-      <c r="B2">
-        <v>2020</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>4</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
-      </c>
-      <c r="F2">
-        <v>154560</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2">
-        <v>30621.84</v>
-      </c>
-      <c r="M2">
-        <v>80291.149999999994</v>
-      </c>
-      <c r="N2">
-        <v>138253.1</v>
-      </c>
-      <c r="O2">
-        <v>136939</v>
-      </c>
-      <c r="P2" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>38</v>
-      </c>
-      <c r="R2" t="s">
-        <v>39</v>
-      </c>
-      <c r="S2" t="s">
-        <v>40</v>
-      </c>
-      <c r="T2">
-        <v>5.6828834647371602</v>
-      </c>
-      <c r="U2">
-        <v>34089.550000000003</v>
-      </c>
-      <c r="V2">
-        <v>76130.009999999995</v>
-      </c>
-      <c r="W2" s="1">
-        <v>115631.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2020</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>5</v>
-      </c>
-      <c r="E3">
-        <v>5</v>
-      </c>
-      <c r="F3">
-        <v>166654</v>
-      </c>
-      <c r="G3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L3">
-        <v>55365</v>
-      </c>
-      <c r="M3">
-        <v>138731.1</v>
-      </c>
-      <c r="N3">
-        <v>152266.70000000001</v>
-      </c>
-      <c r="O3">
-        <v>177573</v>
-      </c>
-      <c r="P3" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>41</v>
-      </c>
-      <c r="R3" t="s">
-        <v>42</v>
-      </c>
-      <c r="S3" t="s">
-        <v>43</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U3">
-        <v>60798.12</v>
-      </c>
-      <c r="V3">
-        <v>146415.79999999999</v>
-      </c>
-      <c r="W3">
-        <v>160521.60000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>2020</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>6</v>
-      </c>
-      <c r="E4">
-        <v>6</v>
-      </c>
-      <c r="F4">
-        <v>188131</v>
-      </c>
-      <c r="G4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4">
-        <v>83170.47</v>
-      </c>
-      <c r="M4">
-        <v>166949.20000000001</v>
-      </c>
-      <c r="N4">
-        <v>171385.1</v>
-      </c>
-      <c r="O4">
-        <v>193397</v>
-      </c>
-      <c r="P4" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>45</v>
-      </c>
-      <c r="R4" t="s">
-        <v>46</v>
-      </c>
-      <c r="S4" t="s">
-        <v>47</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="U4">
-        <v>84951.59</v>
-      </c>
-      <c r="V4">
-        <v>176275.1</v>
-      </c>
-      <c r="W4">
-        <v>172513.3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
       </c>
       <c r="B5">
         <v>2020</v>
@@ -3711,69 +3593,69 @@
         <v>3</v>
       </c>
       <c r="D5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F5">
-        <v>218765</v>
+        <v>154560</v>
       </c>
       <c r="G5" t="s">
         <v>5</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="I5" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="J5" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="L5">
-        <v>71152.070000000007</v>
+        <v>30621.84</v>
       </c>
       <c r="M5">
-        <v>195026</v>
-      </c>
-      <c r="N5" s="1">
-        <v>199844.7</v>
+        <v>80291.149999999994</v>
+      </c>
+      <c r="N5">
+        <v>138253.1</v>
       </c>
       <c r="O5">
-        <v>221563</v>
+        <v>136939</v>
       </c>
       <c r="P5" t="s">
         <v>5</v>
       </c>
       <c r="Q5" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="R5" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="S5" t="s">
-        <v>51</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>52</v>
+        <v>40</v>
+      </c>
+      <c r="T5">
+        <v>5.6828834647371602</v>
       </c>
       <c r="U5">
-        <v>66541.52</v>
+        <v>34089.550000000003</v>
       </c>
       <c r="V5">
-        <v>198746.8</v>
-      </c>
-      <c r="W5">
-        <v>208156.6</v>
+        <v>76130.009999999995</v>
+      </c>
+      <c r="W5" s="1">
+        <v>115631.1</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B6">
         <v>2020</v>
@@ -3782,69 +3664,69 @@
         <v>3</v>
       </c>
       <c r="D6">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E6">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F6">
-        <v>204349</v>
+        <v>166654</v>
       </c>
       <c r="G6" t="s">
         <v>5</v>
       </c>
       <c r="H6" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="I6" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="J6" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="L6">
-        <v>41399.370000000003</v>
+        <v>55365</v>
       </c>
       <c r="M6">
-        <v>143597.70000000001</v>
+        <v>138731.1</v>
       </c>
       <c r="N6">
-        <v>191208.6</v>
+        <v>152266.70000000001</v>
       </c>
       <c r="O6">
-        <v>189968</v>
+        <v>177573</v>
       </c>
       <c r="P6" t="s">
         <v>5</v>
       </c>
       <c r="Q6" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="R6" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="S6" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="U6">
-        <v>45051.519999999997</v>
+        <v>60798.12</v>
       </c>
       <c r="V6">
-        <v>130553</v>
+        <v>146415.79999999999</v>
       </c>
       <c r="W6">
-        <v>174086.39999999999</v>
+        <v>160521.60000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B7">
         <v>2020</v>
@@ -3853,69 +3735,69 @@
         <v>3</v>
       </c>
       <c r="D7">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E7">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F7">
-        <v>126157</v>
+        <v>188131</v>
       </c>
       <c r="G7" t="s">
         <v>5</v>
       </c>
       <c r="H7" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="I7" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="J7" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="L7">
-        <v>22380.79</v>
+        <v>83170.47</v>
       </c>
       <c r="M7">
-        <v>45347.93</v>
+        <v>166949.20000000001</v>
       </c>
       <c r="N7">
-        <v>90978.29</v>
+        <v>171385.1</v>
       </c>
       <c r="O7">
-        <v>137927</v>
+        <v>193397</v>
       </c>
       <c r="P7" t="s">
         <v>5</v>
       </c>
       <c r="Q7" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="R7" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="S7" t="s">
-        <v>59</v>
-      </c>
-      <c r="T7">
-        <v>4.4619556988956397</v>
+        <v>47</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="U7">
-        <v>19428.95</v>
+        <v>84951.59</v>
       </c>
       <c r="V7">
-        <v>39401.769999999997</v>
+        <v>176275.1</v>
       </c>
       <c r="W7">
-        <v>96789.56</v>
+        <v>172513.3</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B8">
         <v>2020</v>
@@ -3924,69 +3806,69 @@
         <v>3</v>
       </c>
       <c r="D8">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E8">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F8">
-        <v>40987</v>
+        <v>218765</v>
       </c>
       <c r="G8" t="s">
         <v>5</v>
       </c>
       <c r="H8" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="I8" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="J8" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="L8">
-        <v>6967.7269999999999</v>
+        <v>71152.070000000007</v>
       </c>
       <c r="M8">
-        <v>9818.83</v>
-      </c>
-      <c r="N8">
-        <v>16842.14</v>
+        <v>195026</v>
+      </c>
+      <c r="N8" s="1">
+        <v>199844.7</v>
       </c>
       <c r="O8">
-        <v>45556</v>
+        <v>221563</v>
       </c>
       <c r="P8" t="s">
         <v>5</v>
       </c>
       <c r="Q8" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="R8" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="S8" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="U8">
-        <v>7432.88</v>
+        <v>66541.52</v>
       </c>
       <c r="V8">
-        <v>11049.76</v>
+        <v>198746.8</v>
       </c>
       <c r="W8">
-        <v>18216.79</v>
+        <v>208156.6</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B9">
         <v>2020</v>
@@ -3995,139 +3877,355 @@
         <v>3</v>
       </c>
       <c r="D9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E9">
-        <v>10</v>
-      </c>
-      <c r="F9" s="2">
-        <v>1099603</v>
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>204349</v>
       </c>
       <c r="G9" t="s">
         <v>5</v>
       </c>
       <c r="H9" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="I9" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="J9" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="L9">
-        <v>312101.2</v>
+        <v>41399.370000000003</v>
       </c>
       <c r="M9">
-        <v>785957.4</v>
-      </c>
-      <c r="N9" s="1">
-        <v>964816.8</v>
-      </c>
-      <c r="O9" s="2">
-        <v>1102923</v>
+        <v>143597.70000000001</v>
+      </c>
+      <c r="N9">
+        <v>191208.6</v>
+      </c>
+      <c r="O9">
+        <v>189968</v>
       </c>
       <c r="P9" t="s">
         <v>5</v>
       </c>
       <c r="Q9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R9" t="s">
+        <v>54</v>
+      </c>
+      <c r="S9" t="s">
+        <v>55</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="U9">
+        <v>45051.519999999997</v>
+      </c>
+      <c r="V9">
+        <v>130553</v>
+      </c>
+      <c r="W9">
+        <v>174086.39999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>2020</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <v>126157</v>
+      </c>
+      <c r="G10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L10">
+        <v>22380.79</v>
+      </c>
+      <c r="M10">
+        <v>45347.93</v>
+      </c>
+      <c r="N10">
+        <v>90978.29</v>
+      </c>
+      <c r="O10">
+        <v>137927</v>
+      </c>
+      <c r="P10" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>57</v>
+      </c>
+      <c r="R10" t="s">
+        <v>58</v>
+      </c>
+      <c r="S10" t="s">
+        <v>59</v>
+      </c>
+      <c r="T10">
+        <v>4.4619556988956397</v>
+      </c>
+      <c r="U10">
+        <v>19428.95</v>
+      </c>
+      <c r="V10">
+        <v>39401.769999999997</v>
+      </c>
+      <c r="W10">
+        <v>96789.56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>2020</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>40987</v>
+      </c>
+      <c r="G11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" t="s">
+        <v>32</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L11">
+        <v>6967.7269999999999</v>
+      </c>
+      <c r="M11">
+        <v>9818.83</v>
+      </c>
+      <c r="N11">
+        <v>16842.14</v>
+      </c>
+      <c r="O11">
+        <v>45556</v>
+      </c>
+      <c r="P11" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>60</v>
+      </c>
+      <c r="R11" t="s">
+        <v>61</v>
+      </c>
+      <c r="S11" t="s">
+        <v>62</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="U11">
+        <v>7432.88</v>
+      </c>
+      <c r="V11">
+        <v>11049.76</v>
+      </c>
+      <c r="W11">
+        <v>18216.79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>2020</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1099603</v>
+      </c>
+      <c r="G12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J12" t="s">
+        <v>36</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L12">
+        <v>312101.2</v>
+      </c>
+      <c r="M12">
+        <v>785957.4</v>
+      </c>
+      <c r="N12" s="1">
+        <v>964816.8</v>
+      </c>
+      <c r="O12" s="2">
+        <v>1102923</v>
+      </c>
+      <c r="P12" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q12" t="s">
         <v>64</v>
       </c>
-      <c r="R9" t="s">
+      <c r="R12" t="s">
         <v>65</v>
       </c>
-      <c r="S9" t="s">
+      <c r="S12" t="s">
         <v>66</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="T12" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="U9">
+      <c r="U12">
         <v>320514</v>
       </c>
-      <c r="V9">
+      <c r="V12">
         <v>774701</v>
       </c>
-      <c r="W9">
+      <c r="W12">
         <v>961573.9</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="21" x14ac:dyDescent="0.35">
-      <c r="D12" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="4">
-        <f>(O9-F9)*100/O9</f>
+    <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D15" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="4">
+        <f>(O12-F12)*100/O12</f>
         <v>0.30101829411482034</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
-        <v>87</v>
-      </c>
-      <c r="E14">
-        <v>2020</v>
-      </c>
-      <c r="F14" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
-        <v>89</v>
-      </c>
-      <c r="E15">
-        <v>312101.2</v>
-      </c>
-      <c r="F15">
-        <v>320514</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
-        <v>90</v>
-      </c>
-      <c r="E16">
-        <v>785957.4</v>
-      </c>
-      <c r="F16">
-        <v>774701</v>
+      <c r="G15" s="3" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E17" s="1">
-        <v>964816.8</v>
-      </c>
-      <c r="F17">
-        <v>961573.9</v>
+        <v>69</v>
+      </c>
+      <c r="E17">
+        <v>2020</v>
+      </c>
+      <c r="F17" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18">
+        <v>312101.2</v>
+      </c>
+      <c r="F18">
+        <v>320514</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19">
+        <v>785957.4</v>
+      </c>
+      <c r="F19">
+        <v>774701</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="1">
+        <v>964816.8</v>
+      </c>
+      <c r="F20">
+        <v>961573.9</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E21" s="2">
         <v>1099603</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F21" s="2">
         <v>1102923</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D12:E12"/>
+  <mergeCells count="3">
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F3:N3"/>
+    <mergeCell ref="O3:W3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>